<commit_message>
novo grafico de pesquisa
</commit_message>
<xml_diff>
--- a/docs/Pesquisa_tcc.xlsx
+++ b/docs/Pesquisa_tcc.xlsx
@@ -1,20 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
-  <workbookPr hidePivotFieldList="1"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22624"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\guipi\Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\git\uniphc\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7C667D85-4A2B-4450-AEC7-D8123512E1E7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{42FF4EBB-A9BE-4DC5-B37F-588271110CF1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha Geral" sheetId="1" r:id="rId1"/>
     <sheet name="Gráfico1" sheetId="8" r:id="rId2"/>
+    <sheet name="Gráfico2" sheetId="11" r:id="rId3"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
@@ -441,34 +442,6 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="17">
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <name val="Calibri"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color rgb="FF000000"/>
-        </left>
-        <right style="thin">
-          <color rgb="FF000000"/>
-        </right>
-        <top/>
-        <bottom/>
-      </border>
-    </dxf>
     <dxf>
       <font>
         <b val="0"/>
@@ -917,13 +890,6 @@
     </dxf>
     <dxf>
       <border outline="0">
-        <bottom style="thin">
-          <color rgb="FF000000"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
         <left style="thin">
           <color rgb="FF000000"/>
         </left>
@@ -936,6 +902,41 @@
         <bottom style="thin">
           <color rgb="FF000000"/>
         </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <bottom style="thin">
+          <color rgb="FF000000"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <name val="Calibri"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color rgb="FF000000"/>
+        </left>
+        <right style="thin">
+          <color rgb="FF000000"/>
+        </right>
+        <top/>
+        <bottom/>
       </border>
     </dxf>
   </dxfs>
@@ -972,7 +973,7 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="1600" b="1" i="0" u="none" strike="noStrike" kern="1200" spc="100" baseline="0">
+              <a:defRPr sz="2000" b="1" i="0" u="none" strike="noStrike" kern="1200" spc="100" baseline="0">
                 <a:solidFill>
                   <a:schemeClr val="lt1">
                     <a:lumMod val="95000"/>
@@ -991,12 +992,20 @@
               </a:defRPr>
             </a:pPr>
             <a:r>
-              <a:rPr lang="pt-BR"/>
-              <a:t>Dificuldades na hora de preencher as horas complementares</a:t>
+              <a:rPr lang="pt-BR" sz="2000" b="1" i="0" baseline="0"/>
+              <a:t>Dificuldades referente as Horas Complementares</a:t>
             </a:r>
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout>
+        <c:manualLayout>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.15127097442332668"/>
+          <c:y val="3.4307890353952868E-2"/>
+        </c:manualLayout>
+      </c:layout>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -1010,7 +1019,7 @@
         <a:lstStyle/>
         <a:p>
           <a:pPr>
-            <a:defRPr sz="1600" b="1" i="0" u="none" strike="noStrike" kern="1200" spc="100" baseline="0">
+            <a:defRPr sz="2000" b="1" i="0" u="none" strike="noStrike" kern="1200" spc="100" baseline="0">
               <a:solidFill>
                 <a:schemeClr val="lt1">
                   <a:lumMod val="95000"/>
@@ -4043,7 +4052,7 @@
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:defRPr sz="2000" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                     <a:solidFill>
                       <a:schemeClr val="lt1">
                         <a:lumMod val="85000"/>
@@ -4167,7 +4176,7 @@
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:defRPr sz="2000" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                     <a:solidFill>
                       <a:schemeClr val="lt1">
                         <a:lumMod val="85000"/>
@@ -4291,7 +4300,7 @@
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:defRPr sz="2000" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                     <a:solidFill>
                       <a:schemeClr val="lt1">
                         <a:lumMod val="85000"/>
@@ -4415,7 +4424,7 @@
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:defRPr sz="2000" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                     <a:solidFill>
                       <a:schemeClr val="lt1">
                         <a:lumMod val="85000"/>
@@ -4539,7 +4548,7 @@
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:defRPr sz="2000" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                     <a:solidFill>
                       <a:schemeClr val="lt1">
                         <a:lumMod val="85000"/>
@@ -4671,7 +4680,7 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:defRPr sz="1600" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
                   <a:schemeClr val="lt1">
                     <a:lumMod val="85000"/>
@@ -4706,7 +4715,7 @@
           <c:x val="5.5804105481697147E-2"/>
           <c:y val="0.90754826026896818"/>
           <c:w val="0.89725784155178645"/>
-          <c:h val="7.9787608866327672E-2"/>
+          <c:h val="8.9878091782108191E-2"/>
         </c:manualLayout>
       </c:layout>
       <c:overlay val="0"/>
@@ -4722,7 +4731,7 @@
         <a:lstStyle/>
         <a:p>
           <a:pPr>
-            <a:defRPr sz="1200" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+            <a:defRPr sz="1800" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
               <a:solidFill>
                 <a:schemeClr val="lt1">
                   <a:lumMod val="85000"/>
@@ -4788,6 +4797,973 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="pt-BR"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="2000" b="1" i="0" u="none" strike="noStrike" kern="1200" spc="100" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="lt1">
+                    <a:lumMod val="95000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:effectLst>
+                  <a:outerShdw blurRad="50800" dist="38100" dir="5400000" algn="t" rotWithShape="0">
+                    <a:prstClr val="black">
+                      <a:alpha val="40000"/>
+                    </a:prstClr>
+                  </a:outerShdw>
+                </a:effectLst>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="pt-BR" sz="2000"/>
+              <a:t>Clareza da instituição sobre</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="pt-BR" sz="2000" baseline="0"/>
+              <a:t> Horas Complementares</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="pt-BR" sz="2000"/>
+              <a:t> </a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="2000" b="1" i="0" u="none" strike="noStrike" kern="1200" spc="100" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="lt1">
+                  <a:lumMod val="95000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:effectLst>
+                <a:outerShdw blurRad="50800" dist="38100" dir="5400000" algn="t" rotWithShape="0">
+                  <a:prstClr val="black">
+                    <a:alpha val="40000"/>
+                  </a:prstClr>
+                </a:outerShdw>
+              </a:effectLst>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="pt-BR"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:pivotFmts>
+      <c:pivotFmt>
+        <c:idx val="0"/>
+        <c:spPr>
+          <a:gradFill rotWithShape="1">
+            <a:gsLst>
+              <a:gs pos="0">
+                <a:schemeClr val="accent2">
+                  <a:satMod val="103000"/>
+                  <a:lumMod val="102000"/>
+                  <a:tint val="94000"/>
+                </a:schemeClr>
+              </a:gs>
+              <a:gs pos="50000">
+                <a:schemeClr val="accent2">
+                  <a:satMod val="110000"/>
+                  <a:lumMod val="100000"/>
+                  <a:shade val="100000"/>
+                </a:schemeClr>
+              </a:gs>
+              <a:gs pos="100000">
+                <a:schemeClr val="accent2">
+                  <a:lumMod val="99000"/>
+                  <a:satMod val="120000"/>
+                  <a:shade val="78000"/>
+                </a:schemeClr>
+              </a:gs>
+            </a:gsLst>
+            <a:lin ang="5400000" scaled="0"/>
+          </a:gradFill>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst>
+            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="63000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+        </c:spPr>
+        <c:marker>
+          <c:spPr>
+            <a:gradFill rotWithShape="1">
+              <a:gsLst>
+                <a:gs pos="0">
+                  <a:schemeClr val="accent2">
+                    <a:satMod val="103000"/>
+                    <a:lumMod val="102000"/>
+                    <a:tint val="94000"/>
+                  </a:schemeClr>
+                </a:gs>
+                <a:gs pos="50000">
+                  <a:schemeClr val="accent2">
+                    <a:satMod val="110000"/>
+                    <a:lumMod val="100000"/>
+                    <a:shade val="100000"/>
+                  </a:schemeClr>
+                </a:gs>
+                <a:gs pos="100000">
+                  <a:schemeClr val="accent2">
+                    <a:lumMod val="99000"/>
+                    <a:satMod val="120000"/>
+                    <a:shade val="78000"/>
+                  </a:schemeClr>
+                </a:gs>
+              </a:gsLst>
+              <a:lin ang="5400000" scaled="0"/>
+            </a:gradFill>
+            <a:ln w="9525">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst>
+              <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+                <a:srgbClr val="000000">
+                  <a:alpha val="63000"/>
+                </a:srgbClr>
+              </a:outerShdw>
+            </a:effectLst>
+          </c:spPr>
+        </c:marker>
+        <c:dLbl>
+          <c:idx val="0"/>
+          <c:dLblPos val="outEnd"/>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="1"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+          </c:extLst>
+        </c:dLbl>
+      </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="1"/>
+        <c:spPr>
+          <a:gradFill rotWithShape="1">
+            <a:gsLst>
+              <a:gs pos="0">
+                <a:schemeClr val="accent2">
+                  <a:satMod val="103000"/>
+                  <a:lumMod val="102000"/>
+                  <a:tint val="94000"/>
+                </a:schemeClr>
+              </a:gs>
+              <a:gs pos="50000">
+                <a:schemeClr val="accent2">
+                  <a:satMod val="110000"/>
+                  <a:lumMod val="100000"/>
+                  <a:shade val="100000"/>
+                </a:schemeClr>
+              </a:gs>
+              <a:gs pos="100000">
+                <a:schemeClr val="accent2">
+                  <a:lumMod val="99000"/>
+                  <a:satMod val="120000"/>
+                  <a:shade val="78000"/>
+                </a:schemeClr>
+              </a:gs>
+            </a:gsLst>
+            <a:lin ang="5400000" scaled="0"/>
+          </a:gradFill>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst>
+            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="63000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+        </c:spPr>
+        <c:marker>
+          <c:symbol val="circle"/>
+          <c:size val="6"/>
+          <c:spPr>
+            <a:gradFill rotWithShape="1">
+              <a:gsLst>
+                <a:gs pos="0">
+                  <a:schemeClr val="accent2">
+                    <a:satMod val="103000"/>
+                    <a:lumMod val="102000"/>
+                    <a:tint val="94000"/>
+                  </a:schemeClr>
+                </a:gs>
+                <a:gs pos="50000">
+                  <a:schemeClr val="accent2">
+                    <a:satMod val="110000"/>
+                    <a:lumMod val="100000"/>
+                    <a:shade val="100000"/>
+                  </a:schemeClr>
+                </a:gs>
+                <a:gs pos="100000">
+                  <a:schemeClr val="accent2">
+                    <a:lumMod val="99000"/>
+                    <a:satMod val="120000"/>
+                    <a:shade val="78000"/>
+                  </a:schemeClr>
+                </a:gs>
+              </a:gsLst>
+              <a:lin ang="5400000" scaled="0"/>
+            </a:gradFill>
+            <a:ln w="9525">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst>
+              <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+                <a:srgbClr val="000000">
+                  <a:alpha val="63000"/>
+                </a:srgbClr>
+              </a:outerShdw>
+            </a:effectLst>
+          </c:spPr>
+        </c:marker>
+        <c:dLbl>
+          <c:idx val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+              <a:spAutoFit/>
+            </a:bodyPr>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="lt1">
+                      <a:lumMod val="85000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="pt-BR"/>
+            </a:p>
+          </c:txPr>
+          <c:dLblPos val="outEnd"/>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="1"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+          </c:extLst>
+        </c:dLbl>
+      </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="2"/>
+        <c:spPr>
+          <a:gradFill rotWithShape="1">
+            <a:gsLst>
+              <a:gs pos="0">
+                <a:schemeClr val="accent2">
+                  <a:satMod val="103000"/>
+                  <a:lumMod val="102000"/>
+                  <a:tint val="94000"/>
+                </a:schemeClr>
+              </a:gs>
+              <a:gs pos="50000">
+                <a:schemeClr val="accent2">
+                  <a:satMod val="110000"/>
+                  <a:lumMod val="100000"/>
+                  <a:shade val="100000"/>
+                </a:schemeClr>
+              </a:gs>
+              <a:gs pos="100000">
+                <a:schemeClr val="accent2">
+                  <a:lumMod val="99000"/>
+                  <a:satMod val="120000"/>
+                  <a:shade val="78000"/>
+                </a:schemeClr>
+              </a:gs>
+            </a:gsLst>
+            <a:lin ang="5400000" scaled="0"/>
+          </a:gradFill>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst>
+            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="63000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+        </c:spPr>
+        <c:marker>
+          <c:symbol val="none"/>
+        </c:marker>
+        <c:dLbl>
+          <c:idx val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+              <a:spAutoFit/>
+            </a:bodyPr>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="lt1">
+                      <a:lumMod val="85000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="pt-BR"/>
+            </a:p>
+          </c:txPr>
+          <c:dLblPos val="outEnd"/>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="1"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+          </c:extLst>
+        </c:dLbl>
+      </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="3"/>
+        <c:spPr>
+          <a:gradFill rotWithShape="1">
+            <a:gsLst>
+              <a:gs pos="0">
+                <a:schemeClr val="accent2">
+                  <a:satMod val="103000"/>
+                  <a:lumMod val="102000"/>
+                  <a:tint val="94000"/>
+                </a:schemeClr>
+              </a:gs>
+              <a:gs pos="50000">
+                <a:schemeClr val="accent2">
+                  <a:satMod val="110000"/>
+                  <a:lumMod val="100000"/>
+                  <a:shade val="100000"/>
+                </a:schemeClr>
+              </a:gs>
+              <a:gs pos="100000">
+                <a:schemeClr val="accent2">
+                  <a:lumMod val="99000"/>
+                  <a:satMod val="120000"/>
+                  <a:shade val="78000"/>
+                </a:schemeClr>
+              </a:gs>
+            </a:gsLst>
+            <a:lin ang="5400000" scaled="0"/>
+          </a:gradFill>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst>
+            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="63000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+        </c:spPr>
+        <c:marker>
+          <c:symbol val="none"/>
+        </c:marker>
+        <c:dLbl>
+          <c:idx val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+              <a:spAutoFit/>
+            </a:bodyPr>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="2000" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="lt1">
+                      <a:lumMod val="85000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="pt-BR"/>
+            </a:p>
+          </c:txPr>
+          <c:dLblPos val="outEnd"/>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="1"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+          </c:extLst>
+        </c:dLbl>
+      </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="4"/>
+        <c:spPr>
+          <a:solidFill>
+            <a:srgbClr val="00B050"/>
+          </a:solidFill>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst>
+            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="63000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+        </c:spPr>
+        <c:marker>
+          <c:symbol val="none"/>
+        </c:marker>
+        <c:dLbl>
+          <c:idx val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+              <a:spAutoFit/>
+            </a:bodyPr>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="2000" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="lt1">
+                      <a:lumMod val="85000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="pt-BR"/>
+            </a:p>
+          </c:txPr>
+          <c:dLblPos val="outEnd"/>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="1"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+          </c:extLst>
+        </c:dLbl>
+      </c:pivotFmt>
+    </c:pivotFmts>
+    <c:plotArea>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="3.060203119484476E-2"/>
+          <c:y val="0.12199742995360487"/>
+          <c:w val="0.95360342555038902"/>
+          <c:h val="0.80121645095605598"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>Ruim</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:gradFill rotWithShape="1">
+              <a:gsLst>
+                <a:gs pos="0">
+                  <a:schemeClr val="accent2">
+                    <a:satMod val="103000"/>
+                    <a:lumMod val="102000"/>
+                    <a:tint val="94000"/>
+                  </a:schemeClr>
+                </a:gs>
+                <a:gs pos="50000">
+                  <a:schemeClr val="accent2">
+                    <a:satMod val="110000"/>
+                    <a:lumMod val="100000"/>
+                    <a:shade val="100000"/>
+                  </a:schemeClr>
+                </a:gs>
+                <a:gs pos="100000">
+                  <a:schemeClr val="accent2">
+                    <a:lumMod val="99000"/>
+                    <a:satMod val="120000"/>
+                    <a:shade val="78000"/>
+                  </a:schemeClr>
+                </a:gs>
+              </a:gsLst>
+              <a:lin ang="5400000" scaled="0"/>
+            </a:gradFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst>
+              <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+                <a:srgbClr val="000000">
+                  <a:alpha val="63000"/>
+                </a:srgbClr>
+              </a:outerShdw>
+            </a:effectLst>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="2000" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="lt1">
+                        <a:lumMod val="85000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="pt-BR"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="outEnd"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525">
+                      <a:solidFill>
+                        <a:schemeClr val="lt1">
+                          <a:lumMod val="95000"/>
+                          <a:alpha val="54000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:cat>
+            <c:strLit>
+              <c:ptCount val="1"/>
+              <c:pt idx="0">
+                <c:v>Total</c:v>
+              </c:pt>
+            </c:strLit>
+          </c:cat>
+          <c:val>
+            <c:numLit>
+              <c:formatCode>General</c:formatCode>
+              <c:ptCount val="1"/>
+              <c:pt idx="0">
+                <c:v>51</c:v>
+              </c:pt>
+            </c:numLit>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-DD10-4C29-A855-3FE23FAF2D2C}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:v>Bom</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="00B050"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst>
+              <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+                <a:srgbClr val="000000">
+                  <a:alpha val="63000"/>
+                </a:srgbClr>
+              </a:outerShdw>
+            </a:effectLst>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="2000" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="lt1">
+                        <a:lumMod val="85000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="pt-BR"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="outEnd"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525">
+                      <a:solidFill>
+                        <a:schemeClr val="lt1">
+                          <a:lumMod val="95000"/>
+                          <a:alpha val="54000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:cat>
+            <c:strLit>
+              <c:ptCount val="1"/>
+              <c:pt idx="0">
+                <c:v>Total</c:v>
+              </c:pt>
+            </c:strLit>
+          </c:cat>
+          <c:val>
+            <c:numLit>
+              <c:formatCode>General</c:formatCode>
+              <c:ptCount val="1"/>
+              <c:pt idx="0">
+                <c:v>32</c:v>
+              </c:pt>
+            </c:numLit>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-DD10-4C29-A855-3FE23FAF2D2C}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="100"/>
+        <c:overlap val="-24"/>
+        <c:axId val="436018304"/>
+        <c:axId val="436018632"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="436018304"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="1"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="436018632"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="436018632"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="lt1">
+                  <a:lumMod val="95000"/>
+                  <a:alpha val="10000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1800" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="lt1">
+                    <a:lumMod val="85000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="pt-BR"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="436018304"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:layout>
+        <c:manualLayout>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="7.0033875357009548E-3"/>
+          <c:y val="0.92201129065389931"/>
+          <c:w val="0.99257428461808417"/>
+          <c:h val="7.7988709346100679E-2"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="2000" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="lt1">
+                  <a:lumMod val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="pt-BR"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:gradFill flip="none" rotWithShape="1">
+      <a:gsLst>
+        <a:gs pos="0">
+          <a:schemeClr val="dk1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:gs>
+        <a:gs pos="100000">
+          <a:schemeClr val="dk1">
+            <a:lumMod val="85000"/>
+            <a:lumOff val="15000"/>
+          </a:schemeClr>
+        </a:gs>
+      </a:gsLst>
+      <a:path path="circle">
+        <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
+      </a:path>
+      <a:tileRect/>
+    </a:gradFill>
+    <a:ln>
+      <a:noFill/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="pt-BR"/>
+    </a:p>
+  </c:txPr>
+  <c:extLst/>
+</c:chartSpace>
+</file>
+
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
@@ -4795,6 +5771,43 @@
   <a:schemeClr val="accent3"/>
   <a:schemeClr val="accent4"/>
   <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="12">
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent4"/>
   <a:schemeClr val="accent6"/>
   <cs:variation/>
   <cs:variation>
@@ -5324,15 +6337,522 @@
 </cs:chartStyle>
 </file>
 
+<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="209">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" b="1" kern="1200" cap="all"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:gradFill flip="none" rotWithShape="1">
+        <a:gsLst>
+          <a:gs pos="0">
+            <a:schemeClr val="dk1">
+              <a:lumMod val="65000"/>
+              <a:lumOff val="35000"/>
+            </a:schemeClr>
+          </a:gs>
+          <a:gs pos="100000">
+            <a:schemeClr val="dk1">
+              <a:lumMod val="85000"/>
+              <a:lumOff val="15000"/>
+            </a:schemeClr>
+          </a:gs>
+        </a:gsLst>
+        <a:path path="circle">
+          <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
+        </a:path>
+        <a:tileRect/>
+      </a:gradFill>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="3">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="3"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="3">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="3"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="3"/>
+    <cs:effectRef idx="3"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="34925" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="3">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="3"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="6"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="3"/>
+    <cs:effectRef idx="3"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:prstDash val="dash"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="10000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="5000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:prstDash val="dash"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="95000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1600" b="1" kern="1200" spc="100" baseline="0">
+      <a:effectLst>
+        <a:outerShdw blurRad="50800" dist="38100" dir="5400000" algn="t" rotWithShape="0">
+          <a:prstClr val="black">
+            <a:alpha val="40000"/>
+          </a:prstClr>
+        </a:outerShdw>
+      </a:effectLst>
+    </cs:defRPr>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
 <file path=xl/chartsheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" xr:uid="{9A150820-FC69-48AC-94AC-3A5CF38E609E}">
   <sheetPr/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="117" workbookViewId="0" zoomToFit="1"/>
+    <sheetView zoomScale="117" workbookViewId="0" zoomToFit="1"/>
   </sheetViews>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="landscape" verticalDpi="300" r:id="rId1"/>
   <drawing r:id="rId2"/>
+</chartsheet>
+</file>
+
+<file path=xl/chartsheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" xr:uid="{D1B3B1B4-8EF7-4D33-A021-955A23A7FD9A}">
+  <sheetPr/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="123" workbookViewId="0" zoomToFit="1"/>
+  </sheetViews>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <drawing r:id="rId1"/>
 </chartsheet>
 </file>
 
@@ -5369,23 +6889,56 @@
 </xdr:wsDr>
 </file>
 
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:absoluteAnchor>
+    <xdr:pos x="0" y="0"/>
+    <xdr:ext cx="9648902" cy="6017012"/>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Gráfico 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A0756B6A-1110-45C4-8BBA-9483C854234C}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks noGrp="1"/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:absoluteAnchor>
+</xdr:wsDr>
+</file>
+
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{9D5194AD-AF0F-4448-A7FC-81425FF423D1}" name="Tabela5" displayName="Tabela5" ref="A1:M84" totalsRowShown="0" headerRowDxfId="0" headerRowBorderDxfId="15" tableBorderDxfId="16" totalsRowBorderDxfId="14">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{9D5194AD-AF0F-4448-A7FC-81425FF423D1}" name="Tabela5" displayName="Tabela5" ref="A1:M84" totalsRowShown="0" headerRowDxfId="16" headerRowBorderDxfId="15" tableBorderDxfId="14" totalsRowBorderDxfId="13">
   <autoFilter ref="A1:M84" xr:uid="{95254A65-5848-44D5-B42C-F732ECA9B417}"/>
   <tableColumns count="13">
-    <tableColumn id="1" xr3:uid="{7836A258-7162-4A31-A0C8-C26E2EC9910F}" name="Data" dataDxfId="13"/>
-    <tableColumn id="2" xr3:uid="{BF24D59C-DE7E-49DB-B78D-D73A1EAFE295}" name="Curso" dataDxfId="12"/>
-    <tableColumn id="3" xr3:uid="{E9040AE2-591A-421B-BEEE-0197E90664CD}" name="Semestre" dataDxfId="11"/>
-    <tableColumn id="4" xr3:uid="{ECEA145E-89C3-4EFE-9826-C56C8E6DDAD5}" name="Faixa Etária" dataDxfId="10"/>
-    <tableColumn id="5" xr3:uid="{DCDAD7A6-3D51-451E-9255-51CBC393C93E}" name="Entendimento das Horas Complementares" dataDxfId="9"/>
-    <tableColumn id="6" xr3:uid="{3EC50C11-B4E9-4583-8236-F911EC235FED}" name="Instituição foi clara" dataDxfId="8"/>
-    <tableColumn id="7" xr3:uid="{3A0C4F80-E652-4F62-9503-4BBCB38A5AC1}" name="Relatório" dataDxfId="7"/>
-    <tableColumn id="8" xr3:uid="{FCFBFADF-735D-4EBA-A93A-F8E5DBE2AC64}" name="Controle das Horas" dataDxfId="6"/>
-    <tableColumn id="9" xr3:uid="{A65136D8-A694-4749-9807-818F0E59C288}" name="Peso das Horas" dataDxfId="5"/>
-    <tableColumn id="10" xr3:uid="{5CC1E7C9-1CAD-47AA-97C5-AFECE3E76DB2}" name="Atividades Válidas" dataDxfId="4"/>
-    <tableColumn id="11" xr3:uid="{43939007-2303-41F1-9054-7B4E57FB5830}" name="Outros" dataDxfId="3"/>
-    <tableColumn id="12" xr3:uid="{431E5466-2574-487D-970E-F8E2B3774587}" name="Utilidade de um app específico" dataDxfId="2"/>
-    <tableColumn id="13" xr3:uid="{E19A83AF-80D2-45D4-8573-AA8031833D6E}" name="Sugestao" dataDxfId="1"/>
+    <tableColumn id="1" xr3:uid="{7836A258-7162-4A31-A0C8-C26E2EC9910F}" name="Data" dataDxfId="12"/>
+    <tableColumn id="2" xr3:uid="{BF24D59C-DE7E-49DB-B78D-D73A1EAFE295}" name="Curso" dataDxfId="11"/>
+    <tableColumn id="3" xr3:uid="{E9040AE2-591A-421B-BEEE-0197E90664CD}" name="Semestre" dataDxfId="10"/>
+    <tableColumn id="4" xr3:uid="{ECEA145E-89C3-4EFE-9826-C56C8E6DDAD5}" name="Faixa Etária" dataDxfId="9"/>
+    <tableColumn id="5" xr3:uid="{DCDAD7A6-3D51-451E-9255-51CBC393C93E}" name="Entendimento das Horas Complementares" dataDxfId="8"/>
+    <tableColumn id="6" xr3:uid="{3EC50C11-B4E9-4583-8236-F911EC235FED}" name="Instituição foi clara" dataDxfId="7"/>
+    <tableColumn id="7" xr3:uid="{3A0C4F80-E652-4F62-9503-4BBCB38A5AC1}" name="Relatório" dataDxfId="6"/>
+    <tableColumn id="8" xr3:uid="{FCFBFADF-735D-4EBA-A93A-F8E5DBE2AC64}" name="Controle das Horas" dataDxfId="5"/>
+    <tableColumn id="9" xr3:uid="{A65136D8-A694-4749-9807-818F0E59C288}" name="Peso das Horas" dataDxfId="4"/>
+    <tableColumn id="10" xr3:uid="{5CC1E7C9-1CAD-47AA-97C5-AFECE3E76DB2}" name="Atividades Válidas" dataDxfId="3"/>
+    <tableColumn id="11" xr3:uid="{43939007-2303-41F1-9054-7B4E57FB5830}" name="Outros" dataDxfId="2"/>
+    <tableColumn id="12" xr3:uid="{431E5466-2574-487D-970E-F8E2B3774587}" name="Utilidade de um app específico" dataDxfId="1"/>
+    <tableColumn id="13" xr3:uid="{E19A83AF-80D2-45D4-8573-AA8031833D6E}" name="Sugestao" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -5595,7 +7148,7 @@
   <dimension ref="A1:M84"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I19" sqref="I19"/>
+      <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>

</xml_diff>